<commit_message>
Primeiro commit com arquivos locais
</commit_message>
<xml_diff>
--- a/aux-enem/mapas/mapa_2019.xlsx
+++ b/aux-enem/mapas/mapa_2019.xlsx
@@ -461,12 +461,12 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>First day of the 2019 exam</t>
+          <t>First day - ENEM 2019</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Second day of the 2019 exam</t>
+          <t>Second day - ENEM 2019</t>
         </is>
       </c>
     </row>
@@ -497,10 +497,10 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>14.42538735603613</v>
+        <v>14.43</v>
       </c>
       <c r="G2" t="n">
-        <v>57.30835096202276</v>
+        <v>18.93</v>
       </c>
     </row>
     <row r="3">
@@ -530,10 +530,10 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>9.324577861163228</v>
+        <v>9.32</v>
       </c>
       <c r="G3" t="n">
-        <v>32.23234624145786</v>
+        <v>13.81</v>
       </c>
     </row>
     <row r="4">
@@ -563,10 +563,10 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>16.49300848278266</v>
+        <v>16.49</v>
       </c>
       <c r="G4" t="n">
-        <v>63.48937583001328</v>
+        <v>21.57</v>
       </c>
     </row>
     <row r="5">
@@ -596,10 +596,10 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>13.98728428701181</v>
+        <v>13.99</v>
       </c>
       <c r="G5" t="n">
-        <v>47.20750101916021</v>
+        <v>20.35</v>
       </c>
     </row>
     <row r="6">
@@ -629,10 +629,10 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>10.26315789473684</v>
+        <v>10.26</v>
       </c>
       <c r="G6" t="n">
-        <v>35.79389289921169</v>
+        <v>13.75</v>
       </c>
     </row>
     <row r="7">
@@ -662,10 +662,10 @@
         </is>
       </c>
       <c r="F7" t="n">
-        <v>10.57864710676447</v>
+        <v>10.58</v>
       </c>
       <c r="G7" t="n">
-        <v>38.90603085553997</v>
+        <v>15.08</v>
       </c>
     </row>
     <row r="8">
@@ -695,10 +695,10 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>11.13678881919225</v>
+        <v>11.14</v>
       </c>
       <c r="G8" t="n">
-        <v>51.90966063615939</v>
+        <v>14.75</v>
       </c>
     </row>
     <row r="9">
@@ -728,10 +728,10 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>12.91383115688799</v>
+        <v>12.91</v>
       </c>
       <c r="G9" t="n">
-        <v>37.90606803555011</v>
+        <v>16.05</v>
       </c>
     </row>
     <row r="10">
@@ -761,10 +761,10 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>9.811555187409402</v>
+        <v>9.81</v>
       </c>
       <c r="G10" t="n">
-        <v>30.61380099123141</v>
+        <v>11.92</v>
       </c>
     </row>
     <row r="11">
@@ -794,10 +794,10 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>17.90353743555955</v>
+        <v>17.9</v>
       </c>
       <c r="G11" t="n">
-        <v>50.04334117602233</v>
+        <v>20.92</v>
       </c>
     </row>
     <row r="12">
@@ -827,10 +827,10 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>8.86530050616738</v>
+        <v>8.869999999999999</v>
       </c>
       <c r="G12" t="n">
-        <v>25.88818315069449</v>
+        <v>11.58</v>
       </c>
     </row>
     <row r="13">
@@ -860,10 +860,10 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>10.07869923528102</v>
+        <v>10.08</v>
       </c>
       <c r="G13" t="n">
-        <v>30.91093117408907</v>
+        <v>12.69</v>
       </c>
     </row>
     <row r="14">
@@ -893,10 +893,10 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>13.2003381783891</v>
+        <v>13.2</v>
       </c>
       <c r="G14" t="n">
-        <v>41.85738604123321</v>
+        <v>16.51</v>
       </c>
     </row>
     <row r="15">
@@ -926,10 +926,10 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>11.68594382086491</v>
+        <v>11.69</v>
       </c>
       <c r="G15" t="n">
-        <v>36.74155695477963</v>
+        <v>14.86</v>
       </c>
     </row>
     <row r="16">
@@ -959,10 +959,10 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>10.15266044167778</v>
+        <v>10.15</v>
       </c>
       <c r="G16" t="n">
-        <v>38.50891708034565</v>
+        <v>12.86</v>
       </c>
     </row>
     <row r="17">
@@ -992,10 +992,10 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>11.68607710137508</v>
+        <v>11.69</v>
       </c>
       <c r="G17" t="n">
-        <v>32.42087435164603</v>
+        <v>15.13</v>
       </c>
     </row>
     <row r="18">
@@ -1025,10 +1025,10 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>11.42244367818217</v>
+        <v>11.42</v>
       </c>
       <c r="G18" t="n">
-        <v>34.33825788253694</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19">
@@ -1058,10 +1058,10 @@
         </is>
       </c>
       <c r="F19" t="n">
-        <v>10.10542050192746</v>
+        <v>10.11</v>
       </c>
       <c r="G19" t="n">
-        <v>34.0517943427982</v>
+        <v>14.17</v>
       </c>
     </row>
     <row r="20">
@@ -1091,10 +1091,10 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>11.10761442156393</v>
+        <v>11.11</v>
       </c>
       <c r="G20" t="n">
-        <v>35.14532700573638</v>
+        <v>15.28</v>
       </c>
     </row>
     <row r="21">
@@ -1124,10 +1124,10 @@
         </is>
       </c>
       <c r="F21" t="n">
-        <v>14.20127242234213</v>
+        <v>14.2</v>
       </c>
       <c r="G21" t="n">
-        <v>41.03407643121609</v>
+        <v>19.16</v>
       </c>
     </row>
     <row r="22">
@@ -1157,10 +1157,10 @@
         </is>
       </c>
       <c r="F22" t="n">
-        <v>14.24566189285444</v>
+        <v>14.25</v>
       </c>
       <c r="G22" t="n">
-        <v>37.49419414770088</v>
+        <v>19.43</v>
       </c>
     </row>
     <row r="23">
@@ -1190,10 +1190,10 @@
         </is>
       </c>
       <c r="F23" t="n">
-        <v>13.47341684465739</v>
+        <v>13.47</v>
       </c>
       <c r="G23" t="n">
-        <v>42.9437767142805</v>
+        <v>18.38</v>
       </c>
     </row>
     <row r="24">
@@ -1223,10 +1223,10 @@
         </is>
       </c>
       <c r="F24" t="n">
-        <v>10.82450782925086</v>
+        <v>10.82</v>
       </c>
       <c r="G24" t="n">
-        <v>36.64126322715061</v>
+        <v>15.34</v>
       </c>
     </row>
     <row r="25">
@@ -1256,10 +1256,10 @@
         </is>
       </c>
       <c r="F25" t="n">
-        <v>10.663491859193</v>
+        <v>10.66</v>
       </c>
       <c r="G25" t="n">
-        <v>41.14420723989537</v>
+        <v>15.14</v>
       </c>
     </row>
     <row r="26">
@@ -1289,10 +1289,10 @@
         </is>
       </c>
       <c r="F26" t="n">
-        <v>11.93541227388747</v>
+        <v>11.94</v>
       </c>
       <c r="G26" t="n">
-        <v>40.32302030802781</v>
+        <v>16.51</v>
       </c>
     </row>
     <row r="27">
@@ -1322,10 +1322,10 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>10.40934027289352</v>
+        <v>10.41</v>
       </c>
       <c r="G27" t="n">
-        <v>49.85038597902889</v>
+        <v>14.05</v>
       </c>
     </row>
     <row r="28">
@@ -1355,10 +1355,10 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>8.166073546856465</v>
+        <v>8.17</v>
       </c>
       <c r="G28" t="n">
-        <v>27.86290322580645</v>
+        <v>11.29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>